<commit_message>
Scenery tweaks (2) and info
</commit_message>
<xml_diff>
--- a/objectInfo.xlsx
+++ b/objectInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Usuarios\Chris\Documentos\GitHub\wind-turbine-vr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A4753F-BCF5-42F7-B2E4-E8ADCF422BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE48A388-69CE-4BA4-B6CA-38729643C97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6630" yWindow="1890" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Veleta</t>
   </si>
@@ -33,7 +33,25 @@
     <t>Dispositivo que capta la dirección del viento. Esta dirección es leída por el ordenador de control varias veces por minuto, activando el sistema de orientación.</t>
   </si>
   <si>
-    <t>Veleta | Darrera</t>
+    <t>wind-energie.de/themen/anlagentechnik/konstruktiver-aufbau/maschinenhaus/</t>
+  </si>
+  <si>
+    <t>https://www.darrera.com/wp/es/producto/14567-veleta/</t>
+  </si>
+  <si>
+    <t>Freno Hidráulico</t>
+  </si>
+  <si>
+    <t>El freno hidráulico se encarga de detener el movimiento del rotor de forma secundaria.</t>
+  </si>
+  <si>
+    <t>Esto significa que no es el principal mecanismo de frenado, sino que asiste al frenado mediante el uso de las palas.</t>
+  </si>
+  <si>
+    <t>Eje rápido</t>
+  </si>
+  <si>
+    <t>El eje rápido conecta la multiplicadora con el generador eléctrico, transmitiendo la rotación tras haber sido convertida.</t>
   </si>
 </sst>
 </file>
@@ -65,7 +83,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -73,14 +91,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -362,29 +401,262 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="20.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" display="https://www.darrera.com/wp/es/producto/14567-veleta/" xr:uid="{CF65BB7F-EE3C-42B1-8FFD-094F67897A4F}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.wind-energie.de/themen/anlagentechnik/konstruktiver-aufbau/maschinenhaus/" xr:uid="{4734B221-3C5D-43FC-BAB8-AD70CE5D9BE7}"/>
+    <hyperlink ref="B1" r:id="rId2" xr:uid="{A2E8F67E-1158-4B89-B199-8EA938AD88EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Highlight and Anemometer (1)
</commit_message>
<xml_diff>
--- a/objectInfo.xlsx
+++ b/objectInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Usuarios\Chris\Documentos\GitHub\wind-turbine-vr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE48A388-69CE-4BA4-B6CA-38729643C97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAFC98F-69BC-4CAD-B70F-C0B3B28BF98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6630" yWindow="1890" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -404,7 +404,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Info, UI & Teleport
Generator info
UI renders on top of everything else
Teleport info panels hide when far and show up when close.
</commit_message>
<xml_diff>
--- a/objectInfo.xlsx
+++ b/objectInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Usuarios\Chris\Documentos\GitHub\wind-turbine-vr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48162552-C372-497E-87BB-1444EFE43D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD45DDE-A0F5-4FA4-8F4D-A417D67D61F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8145" yWindow="3060" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Veleta</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t>Es el encargado de rotar la góndola para que esté de forma paralela a la dirección del viento.</t>
+  </si>
+  <si>
+    <t>Generador</t>
+  </si>
+  <si>
+    <t>Alternador para aerogenerador - Duplex - CRRC ZHUZHOU ELECTRIC CO., LTD - trifásico / para generador / con refrigeración por líquido (directindustry.es)</t>
+  </si>
+  <si>
+    <t>27. Generador asíncrono jaula de ardilla para aerogeneradores Fuente:... | Download Scientific Diagram (researchgate.net)</t>
+  </si>
+  <si>
+    <t>Es el dispositivo encargado de convertir la energía mecánica rotacional en energía eléctrica.</t>
   </si>
 </sst>
 </file>
@@ -169,15 +181,19 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -464,284 +480,295 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="14" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="3" t="s">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="4" t="s">
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -750,8 +777,10 @@
     <hyperlink ref="I5" r:id="rId3" xr:uid="{E16F6EDE-C3EF-4CE5-8F37-DD259B140ACE}"/>
     <hyperlink ref="J5" r:id="rId4" display="https://www.schaeffler.es/es/productos-y-soluciones/industria/soluciones-sectoriales/energia/energia-eolica/multiplicadora/" xr:uid="{92C784D8-24BD-4977-99D8-C6FF164440B0}"/>
     <hyperlink ref="I7" r:id="rId5" display="https://www.br-automation.com/es/sobre-nosotros/customer-magazine/2016/20169/potencial-sustancial-para-optimizar-el-control-del-azimut/" xr:uid="{A21BFC50-FC27-4D74-9D4C-21DFE68A39D8}"/>
+    <hyperlink ref="J8" r:id="rId6" display="https://www.directindustry.es/prod/crrc-zhuzhou-electric-co-ltd/product-162644-1757009.html" xr:uid="{1265E041-8818-448D-8AB4-BE0A6B11A872}"/>
+    <hyperlink ref="I8" r:id="rId7" display="https://www.researchgate.net/figure/Figura-227-Generador-asincrono-jaula-de-ardilla-para-aerogeneradores-Fuente_fig9_281903643" xr:uid="{5CA9B4BD-2B46-4707-9CA0-B692563ECF54}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Wind turbine info panel
</commit_message>
<xml_diff>
--- a/objectInfo.xlsx
+++ b/objectInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Usuarios\Chris\Documentos\GitHub\wind-turbine-vr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD45DDE-A0F5-4FA4-8F4D-A417D67D61F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AD76B3-E500-416C-AA5A-6FA4589F6095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8145" yWindow="3060" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="2700" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Veleta</t>
   </si>
@@ -109,6 +109,21 @@
   </si>
   <si>
     <t>Es el dispositivo encargado de convertir la energía mecánica rotacional en energía eléctrica.</t>
+  </si>
+  <si>
+    <t>Aerogenerador</t>
+  </si>
+  <si>
+    <t>Un aerogenerador es un dispositivo que convierte la energía cinética del viento en energía eléctrica que podemos utilizar.</t>
+  </si>
+  <si>
+    <t>Esto lo consigue mediante el uso de componentes como las aspas, el rotor, una multiplicadora y un generador eléctrico.</t>
+  </si>
+  <si>
+    <t>Existen diferentes tipos de aerogeneradores según su forma, su potencia, su generador, etc…</t>
+  </si>
+  <si>
+    <t>En nuestro caso, estamos ante un HAWT (Horizontal Axis Wind Turbine), up-wind (que recibe el viento de frente) situado en tierra firme.</t>
   </si>
 </sst>
 </file>
@@ -480,7 +495,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,12 +646,22 @@
       </c>
     </row>
     <row r="9" spans="1:10" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>

</xml_diff>